<commit_message>
handling raid_tiers and multiple args in each cmd. read_data now sets sheet name based on the raid tier selected
</commit_message>
<xml_diff>
--- a/data/20230805_prio.xlsx
+++ b/data/20230805_prio.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamh\OneDrive\Desktop\python\RelsieBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EABF35-B1D2-47FD-AA09-4F620858030B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DFF2DB-538A-4D3D-ADB0-3741E9F84C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{5F1516B2-90AE-4783-A0A2-8D6006BEDECA}"/>
+    <workbookView xWindow="2580" yWindow="600" windowWidth="16457" windowHeight="9506" activeTab="1" xr2:uid="{5F1516B2-90AE-4783-A0A2-8D6006BEDECA}"/>
   </bookViews>
   <sheets>
-    <sheet name="TOGC" sheetId="1" r:id="rId1"/>
-    <sheet name="Ulduar" sheetId="2" r:id="rId2"/>
+    <sheet name="togc" sheetId="1" r:id="rId1"/>
+    <sheet name="ulduar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4110,15 +4110,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
@@ -4129,6 +4120,15 @@
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4456,18 +4456,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8116F2-EA76-428C-8F61-233936A21BFD}">
   <dimension ref="A1:FM104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:169" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:169" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:169" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4638,7 +4638,7 @@
       <c r="FL2" s="3"/>
       <c r="FM2" s="3"/>
     </row>
-    <row r="3" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4809,20 +4809,20 @@
       <c r="FL3" s="7"/>
       <c r="FM3" s="7"/>
     </row>
-    <row r="4" spans="1:169" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:169" ht="45.9" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -4982,7 +4982,7 @@
       <c r="FL4" s="7"/>
       <c r="FM4" s="7"/>
     </row>
-    <row r="5" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -5153,7 +5153,7 @@
       <c r="FL5" s="7"/>
       <c r="FM5" s="7"/>
     </row>
-    <row r="6" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:169" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -5324,7 +5324,7 @@
       <c r="FL6" s="9"/>
       <c r="FM6" s="9"/>
     </row>
-    <row r="7" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -5497,7 +5497,7 @@
       <c r="FL7" s="11"/>
       <c r="FM7" s="11"/>
     </row>
-    <row r="8" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="12" t="s">
@@ -5680,7 +5680,7 @@
       <c r="FL8" s="11"/>
       <c r="FM8" s="11"/>
     </row>
-    <row r="9" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5853,7 +5853,7 @@
       <c r="FL9" s="11"/>
       <c r="FM9" s="11"/>
     </row>
-    <row r="10" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -6046,7 +6046,7 @@
       <c r="FL10" s="11"/>
       <c r="FM10" s="11"/>
     </row>
-    <row r="11" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -6225,7 +6225,7 @@
       <c r="FL11" s="11"/>
       <c r="FM11" s="11"/>
     </row>
-    <row r="12" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -6400,7 +6400,7 @@
       <c r="FL12" s="11"/>
       <c r="FM12" s="11"/>
     </row>
-    <row r="13" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -6573,7 +6573,7 @@
       <c r="FL13" s="11"/>
       <c r="FM13" s="11"/>
     </row>
-    <row r="14" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -6750,7 +6750,7 @@
       <c r="FL14" s="11"/>
       <c r="FM14" s="11"/>
     </row>
-    <row r="15" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -6933,7 +6933,7 @@
       <c r="FL15" s="11"/>
       <c r="FM15" s="11"/>
     </row>
-    <row r="16" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -7120,7 +7120,7 @@
       <c r="FL16" s="11"/>
       <c r="FM16" s="11"/>
     </row>
-    <row r="17" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -7299,7 +7299,7 @@
       <c r="FL17" s="11"/>
       <c r="FM17" s="11"/>
     </row>
-    <row r="18" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -7478,7 +7478,7 @@
       <c r="FL18" s="11"/>
       <c r="FM18" s="11"/>
     </row>
-    <row r="19" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -7661,7 +7661,7 @@
       <c r="FL19" s="11"/>
       <c r="FM19" s="11"/>
     </row>
-    <row r="20" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="12" t="s">
@@ -7842,7 +7842,7 @@
       <c r="FL20" s="11"/>
       <c r="FM20" s="11"/>
     </row>
-    <row r="21" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -8025,7 +8025,7 @@
       <c r="FL21" s="11"/>
       <c r="FM21" s="11"/>
     </row>
-    <row r="22" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -8202,7 +8202,7 @@
       <c r="FL22" s="11"/>
       <c r="FM22" s="11"/>
     </row>
-    <row r="23" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -8387,7 +8387,7 @@
       <c r="FL23" s="11"/>
       <c r="FM23" s="11"/>
     </row>
-    <row r="24" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -8560,7 +8560,7 @@
       <c r="FL24" s="11"/>
       <c r="FM24" s="11"/>
     </row>
-    <row r="25" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -8735,7 +8735,7 @@
       <c r="FL25" s="11"/>
       <c r="FM25" s="11"/>
     </row>
-    <row r="26" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -8926,7 +8926,7 @@
       <c r="FL26" s="11"/>
       <c r="FM26" s="11"/>
     </row>
-    <row r="27" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -9105,7 +9105,7 @@
       <c r="FL27" s="11"/>
       <c r="FM27" s="11"/>
     </row>
-    <row r="28" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -9288,7 +9288,7 @@
       <c r="FL28" s="11"/>
       <c r="FM28" s="11"/>
     </row>
-    <row r="29" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -9467,7 +9467,7 @@
       <c r="FL29" s="11"/>
       <c r="FM29" s="11"/>
     </row>
-    <row r="30" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -9646,7 +9646,7 @@
       <c r="FL30" s="11"/>
       <c r="FM30" s="11"/>
     </row>
-    <row r="31" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -9821,7 +9821,7 @@
       <c r="FL31" s="11"/>
       <c r="FM31" s="11"/>
     </row>
-    <row r="32" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -10000,7 +10000,7 @@
       <c r="FL32" s="11"/>
       <c r="FM32" s="11"/>
     </row>
-    <row r="33" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="12" t="s">
@@ -10175,7 +10175,7 @@
       <c r="FL33" s="11"/>
       <c r="FM33" s="11"/>
     </row>
-    <row r="34" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -10358,7 +10358,7 @@
       <c r="FL34" s="11"/>
       <c r="FM34" s="11"/>
     </row>
-    <row r="35" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -10539,7 +10539,7 @@
       <c r="FL35" s="11"/>
       <c r="FM35" s="11"/>
     </row>
-    <row r="36" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -10728,7 +10728,7 @@
       <c r="FL36" s="11"/>
       <c r="FM36" s="11"/>
     </row>
-    <row r="37" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -10907,7 +10907,7 @@
       <c r="FL37" s="11"/>
       <c r="FM37" s="11"/>
     </row>
-    <row r="38" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -11086,7 +11086,7 @@
       <c r="FL38" s="11"/>
       <c r="FM38" s="11"/>
     </row>
-    <row r="39" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -11281,7 +11281,7 @@
       <c r="FL39" s="11"/>
       <c r="FM39" s="11"/>
     </row>
-    <row r="40" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -11456,7 +11456,7 @@
       <c r="FL40" s="11"/>
       <c r="FM40" s="11"/>
     </row>
-    <row r="41" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -11633,7 +11633,7 @@
       <c r="FL41" s="11"/>
       <c r="FM41" s="11"/>
     </row>
-    <row r="42" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -11810,7 +11810,7 @@
       <c r="FL42" s="11"/>
       <c r="FM42" s="11"/>
     </row>
-    <row r="43" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -11997,7 +11997,7 @@
       <c r="FL43" s="11"/>
       <c r="FM43" s="11"/>
     </row>
-    <row r="44" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -12188,7 +12188,7 @@
       <c r="FL44" s="11"/>
       <c r="FM44" s="11"/>
     </row>
-    <row r="45" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -12375,7 +12375,7 @@
       <c r="FL45" s="11"/>
       <c r="FM45" s="11"/>
     </row>
-    <row r="46" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -12562,7 +12562,7 @@
       <c r="FL46" s="11"/>
       <c r="FM46" s="11"/>
     </row>
-    <row r="47" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -12735,7 +12735,7 @@
       <c r="FL47" s="11"/>
       <c r="FM47" s="11"/>
     </row>
-    <row r="48" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -12924,7 +12924,7 @@
       <c r="FL48" s="11"/>
       <c r="FM48" s="11"/>
     </row>
-    <row r="49" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -13109,7 +13109,7 @@
       <c r="FL49" s="11"/>
       <c r="FM49" s="11"/>
     </row>
-    <row r="50" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="4"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -13292,7 +13292,7 @@
       <c r="FL50" s="11"/>
       <c r="FM50" s="11"/>
     </row>
-    <row r="51" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -13467,7 +13467,7 @@
       <c r="FL51" s="11"/>
       <c r="FM51" s="11"/>
     </row>
-    <row r="52" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -13640,7 +13640,7 @@
       <c r="FL52" s="11"/>
       <c r="FM52" s="11"/>
     </row>
-    <row r="53" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="4"/>
       <c r="B53" s="5"/>
       <c r="C53" s="12" t="s">
@@ -13829,7 +13829,7 @@
       <c r="FL53" s="11"/>
       <c r="FM53" s="11"/>
     </row>
-    <row r="54" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" s="4"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -14012,7 +14012,7 @@
       <c r="FL54" s="11"/>
       <c r="FM54" s="11"/>
     </row>
-    <row r="55" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -14197,7 +14197,7 @@
       <c r="FL55" s="11"/>
       <c r="FM55" s="11"/>
     </row>
-    <row r="56" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -14372,7 +14372,7 @@
       <c r="FL56" s="11"/>
       <c r="FM56" s="11"/>
     </row>
-    <row r="57" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -14555,7 +14555,7 @@
       <c r="FL57" s="11"/>
       <c r="FM57" s="11"/>
     </row>
-    <row r="58" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -14730,7 +14730,7 @@
       <c r="FL58" s="11"/>
       <c r="FM58" s="11"/>
     </row>
-    <row r="59" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -14927,7 +14927,7 @@
       <c r="FL59" s="11"/>
       <c r="FM59" s="11"/>
     </row>
-    <row r="60" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -15102,7 +15102,7 @@
       <c r="FL60" s="11"/>
       <c r="FM60" s="11"/>
     </row>
-    <row r="61" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -15275,7 +15275,7 @@
       <c r="FL61" s="11"/>
       <c r="FM61" s="11"/>
     </row>
-    <row r="62" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A62" s="4"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -15448,7 +15448,7 @@
       <c r="FL62" s="11"/>
       <c r="FM62" s="11"/>
     </row>
-    <row r="63" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="4"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -15635,7 +15635,7 @@
       <c r="FL63" s="11"/>
       <c r="FM63" s="11"/>
     </row>
-    <row r="64" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -15820,7 +15820,7 @@
       <c r="FL64" s="11"/>
       <c r="FM64" s="11"/>
     </row>
-    <row r="65" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -15999,7 +15999,7 @@
       <c r="FL65" s="11"/>
       <c r="FM65" s="11"/>
     </row>
-    <row r="66" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="4"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -16178,7 +16178,7 @@
       <c r="FL66" s="11"/>
       <c r="FM66" s="11"/>
     </row>
-    <row r="67" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -16381,7 +16381,7 @@
       <c r="FL67" s="11"/>
       <c r="FM67" s="11"/>
     </row>
-    <row r="68" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="12" t="s">
@@ -16564,7 +16564,7 @@
       <c r="FL68" s="11"/>
       <c r="FM68" s="11"/>
     </row>
-    <row r="69" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A69" s="4"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -16753,7 +16753,7 @@
       <c r="FL69" s="11"/>
       <c r="FM69" s="11"/>
     </row>
-    <row r="70" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A70" s="4"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -16950,7 +16950,7 @@
       <c r="FL70" s="11"/>
       <c r="FM70" s="11"/>
     </row>
-    <row r="71" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -17127,7 +17127,7 @@
       <c r="FL71" s="11"/>
       <c r="FM71" s="11"/>
     </row>
-    <row r="72" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A72" s="4"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -17300,7 +17300,7 @@
       <c r="FL72" s="11"/>
       <c r="FM72" s="11"/>
     </row>
-    <row r="73" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="4"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -17479,7 +17479,7 @@
       <c r="FL73" s="11"/>
       <c r="FM73" s="11"/>
     </row>
-    <row r="74" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -17652,7 +17652,7 @@
       <c r="FL74" s="11"/>
       <c r="FM74" s="11"/>
     </row>
-    <row r="75" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A75" s="4"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -17835,7 +17835,7 @@
       <c r="FL75" s="11"/>
       <c r="FM75" s="11"/>
     </row>
-    <row r="76" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="4"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -18016,7 +18016,7 @@
       <c r="FL76" s="11"/>
       <c r="FM76" s="11"/>
     </row>
-    <row r="77" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -18195,7 +18195,7 @@
       <c r="FL77" s="11"/>
       <c r="FM77" s="11"/>
     </row>
-    <row r="78" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -18376,7 +18376,7 @@
       <c r="FL78" s="11"/>
       <c r="FM78" s="11"/>
     </row>
-    <row r="79" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -18553,7 +18553,7 @@
       <c r="FL79" s="11"/>
       <c r="FM79" s="11"/>
     </row>
-    <row r="80" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -18728,7 +18728,7 @@
       <c r="FL80" s="11"/>
       <c r="FM80" s="11"/>
     </row>
-    <row r="81" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A81" s="4"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -18909,7 +18909,7 @@
       <c r="FL81" s="11"/>
       <c r="FM81" s="11"/>
     </row>
-    <row r="82" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -19084,7 +19084,7 @@
       <c r="FL82" s="11"/>
       <c r="FM82" s="11"/>
     </row>
-    <row r="83" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -19265,7 +19265,7 @@
       <c r="FL83" s="11"/>
       <c r="FM83" s="11"/>
     </row>
-    <row r="84" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -19454,7 +19454,7 @@
       <c r="FL84" s="11"/>
       <c r="FM84" s="11"/>
     </row>
-    <row r="85" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A85" s="4"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -19635,7 +19635,7 @@
       <c r="FL85" s="11"/>
       <c r="FM85" s="11"/>
     </row>
-    <row r="86" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -19826,7 +19826,7 @@
       <c r="FL86" s="11"/>
       <c r="FM86" s="11"/>
     </row>
-    <row r="87" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -20003,7 +20003,7 @@
       <c r="FL87" s="11"/>
       <c r="FM87" s="11"/>
     </row>
-    <row r="88" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="25" t="s">
@@ -20194,7 +20194,7 @@
       <c r="FL88" s="11"/>
       <c r="FM88" s="11"/>
     </row>
-    <row r="89" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -20373,7 +20373,7 @@
       <c r="FL89" s="11"/>
       <c r="FM89" s="11"/>
     </row>
-    <row r="90" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -20554,7 +20554,7 @@
       <c r="FL90" s="11"/>
       <c r="FM90" s="11"/>
     </row>
-    <row r="91" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -20743,7 +20743,7 @@
       <c r="FL91" s="11"/>
       <c r="FM91" s="11"/>
     </row>
-    <row r="92" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -20930,7 +20930,7 @@
       <c r="FL92" s="11"/>
       <c r="FM92" s="11"/>
     </row>
-    <row r="93" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -21107,7 +21107,7 @@
       <c r="FL93" s="11"/>
       <c r="FM93" s="11"/>
     </row>
-    <row r="94" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A94" s="4"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -21288,7 +21288,7 @@
       <c r="FL94" s="11"/>
       <c r="FM94" s="11"/>
     </row>
-    <row r="95" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="25" t="s">
@@ -21473,7 +21473,7 @@
       <c r="FL95" s="11"/>
       <c r="FM95" s="11"/>
     </row>
-    <row r="96" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A96" s="4"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -21676,7 +21676,7 @@
       <c r="FL96" s="11"/>
       <c r="FM96" s="11"/>
     </row>
-    <row r="97" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="4"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -21861,7 +21861,7 @@
       <c r="FL97" s="11"/>
       <c r="FM97" s="11"/>
     </row>
-    <row r="98" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -22048,7 +22048,7 @@
       <c r="FL98" s="11"/>
       <c r="FM98" s="11"/>
     </row>
-    <row r="99" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A99" s="4"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -22229,7 +22229,7 @@
       <c r="FL99" s="11"/>
       <c r="FM99" s="11"/>
     </row>
-    <row r="100" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
       <c r="C100" s="25" t="s">
@@ -22482,7 +22482,7 @@
       <c r="FL100" s="11"/>
       <c r="FM100" s="11"/>
     </row>
-    <row r="101" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -22719,7 +22719,7 @@
       <c r="FL101" s="11"/>
       <c r="FM101" s="11"/>
     </row>
-    <row r="102" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -22998,7 +22998,7 @@
       <c r="FL102" s="11"/>
       <c r="FM102" s="11"/>
     </row>
-    <row r="103" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -23169,7 +23169,7 @@
       <c r="FL103" s="26"/>
       <c r="FM103" s="26"/>
     </row>
-    <row r="104" spans="1:169" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:169" ht="154.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A104" s="27" t="s">
         <v>551</v>
       </c>
@@ -23187,18 +23187,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CC7423-408E-4855-AD71-F153B034110D}">
   <dimension ref="A1:FM253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:169" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:169" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:169" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -23369,7 +23369,7 @@
       <c r="FL2" s="3"/>
       <c r="FM2" s="3"/>
     </row>
-    <row r="3" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -23540,7 +23540,7 @@
       <c r="FL3" s="7"/>
       <c r="FM3" s="7"/>
     </row>
-    <row r="4" spans="1:169" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:169" ht="45.9" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="35" t="s">
@@ -23713,7 +23713,7 @@
       <c r="FL4" s="7"/>
       <c r="FM4" s="7"/>
     </row>
-    <row r="5" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -23884,7 +23884,7 @@
       <c r="FL5" s="7"/>
       <c r="FM5" s="7"/>
     </row>
-    <row r="6" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:169" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -24055,10 +24055,10 @@
       <c r="FL6" s="9"/>
       <c r="FM6" s="9"/>
     </row>
-    <row r="7" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="28" t="s">
         <v>553</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -24236,7 +24236,7 @@
       <c r="FL7" s="11"/>
       <c r="FM7" s="11"/>
     </row>
-    <row r="8" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -24411,7 +24411,7 @@
       <c r="FL8" s="11"/>
       <c r="FM8" s="11"/>
     </row>
-    <row r="9" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -24584,7 +24584,7 @@
       <c r="FL9" s="11"/>
       <c r="FM9" s="11"/>
     </row>
-    <row r="10" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -24757,7 +24757,7 @@
       <c r="FL10" s="11"/>
       <c r="FM10" s="11"/>
     </row>
-    <row r="11" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -24930,7 +24930,7 @@
       <c r="FL11" s="11"/>
       <c r="FM11" s="11"/>
     </row>
-    <row r="12" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -25103,7 +25103,7 @@
       <c r="FL12" s="11"/>
       <c r="FM12" s="11"/>
     </row>
-    <row r="13" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -25278,7 +25278,7 @@
       <c r="FL13" s="11"/>
       <c r="FM13" s="11"/>
     </row>
-    <row r="14" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -25459,7 +25459,7 @@
       <c r="FL14" s="11"/>
       <c r="FM14" s="11"/>
     </row>
-    <row r="15" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -25632,7 +25632,7 @@
       <c r="FL15" s="11"/>
       <c r="FM15" s="11"/>
     </row>
-    <row r="16" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -25809,7 +25809,7 @@
       <c r="FL16" s="11"/>
       <c r="FM16" s="11"/>
     </row>
-    <row r="17" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -25982,7 +25982,7 @@
       <c r="FL17" s="11"/>
       <c r="FM17" s="11"/>
     </row>
-    <row r="18" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -26155,10 +26155,10 @@
       <c r="FL18" s="11"/>
       <c r="FM18" s="11"/>
     </row>
-    <row r="19" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="28" t="s">
         <v>575</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -26330,7 +26330,7 @@
       <c r="FL19" s="11"/>
       <c r="FM19" s="11"/>
     </row>
-    <row r="20" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -26503,7 +26503,7 @@
       <c r="FL20" s="11"/>
       <c r="FM20" s="11"/>
     </row>
-    <row r="21" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -26676,7 +26676,7 @@
       <c r="FL21" s="11"/>
       <c r="FM21" s="11"/>
     </row>
-    <row r="22" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -26849,7 +26849,7 @@
       <c r="FL22" s="11"/>
       <c r="FM22" s="11"/>
     </row>
-    <row r="23" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -27022,7 +27022,7 @@
       <c r="FL23" s="11"/>
       <c r="FM23" s="11"/>
     </row>
-    <row r="24" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -27195,7 +27195,7 @@
       <c r="FL24" s="11"/>
       <c r="FM24" s="11"/>
     </row>
-    <row r="25" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -27376,7 +27376,7 @@
       <c r="FL25" s="11"/>
       <c r="FM25" s="11"/>
     </row>
-    <row r="26" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -27553,7 +27553,7 @@
       <c r="FL26" s="11"/>
       <c r="FM26" s="11"/>
     </row>
-    <row r="27" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -27728,7 +27728,7 @@
       <c r="FL27" s="11"/>
       <c r="FM27" s="11"/>
     </row>
-    <row r="28" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -27901,7 +27901,7 @@
       <c r="FL28" s="11"/>
       <c r="FM28" s="11"/>
     </row>
-    <row r="29" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -28074,7 +28074,7 @@
       <c r="FL29" s="11"/>
       <c r="FM29" s="11"/>
     </row>
-    <row r="30" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -28247,7 +28247,7 @@
       <c r="FL30" s="11"/>
       <c r="FM30" s="11"/>
     </row>
-    <row r="31" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -28428,7 +28428,7 @@
       <c r="FL31" s="11"/>
       <c r="FM31" s="11"/>
     </row>
-    <row r="32" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -28601,7 +28601,7 @@
       <c r="FL32" s="11"/>
       <c r="FM32" s="11"/>
     </row>
-    <row r="33" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -28774,13 +28774,13 @@
       <c r="FL33" s="11"/>
       <c r="FM33" s="11"/>
     </row>
-    <row r="34" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="30" t="s">
         <v>601</v>
       </c>
       <c r="E34" s="6"/>
@@ -28965,11 +28965,11 @@
       <c r="FL34" s="11"/>
       <c r="FM34" s="11"/>
     </row>
-    <row r="35" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="30" t="s">
         <v>608</v>
       </c>
       <c r="E35" s="6"/>
@@ -29140,11 +29140,11 @@
       <c r="FL35" s="11"/>
       <c r="FM35" s="11"/>
     </row>
-    <row r="36" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="30" t="s">
         <v>610</v>
       </c>
       <c r="E36" s="6"/>
@@ -29325,11 +29325,11 @@
       <c r="FL36" s="11"/>
       <c r="FM36" s="11"/>
     </row>
-    <row r="37" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="30" t="s">
         <v>617</v>
       </c>
       <c r="E37" s="6"/>
@@ -29520,11 +29520,11 @@
       <c r="FL37" s="11"/>
       <c r="FM37" s="11"/>
     </row>
-    <row r="38" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="30" t="s">
         <v>626</v>
       </c>
       <c r="E38" s="6"/>
@@ -29695,10 +29695,10 @@
       <c r="FL38" s="11"/>
       <c r="FM38" s="11"/>
     </row>
-    <row r="39" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="28" t="s">
         <v>628</v>
       </c>
       <c r="D39" s="10" t="s">
@@ -29872,7 +29872,7 @@
       <c r="FL39" s="11"/>
       <c r="FM39" s="11"/>
     </row>
-    <row r="40" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -30045,7 +30045,7 @@
       <c r="FL40" s="11"/>
       <c r="FM40" s="11"/>
     </row>
-    <row r="41" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -30218,7 +30218,7 @@
       <c r="FL41" s="11"/>
       <c r="FM41" s="11"/>
     </row>
-    <row r="42" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -30393,7 +30393,7 @@
       <c r="FL42" s="11"/>
       <c r="FM42" s="11"/>
     </row>
-    <row r="43" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -30566,7 +30566,7 @@
       <c r="FL43" s="11"/>
       <c r="FM43" s="11"/>
     </row>
-    <row r="44" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -30749,7 +30749,7 @@
       <c r="FL44" s="11"/>
       <c r="FM44" s="11"/>
     </row>
-    <row r="45" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -30924,7 +30924,7 @@
       <c r="FL45" s="11"/>
       <c r="FM45" s="11"/>
     </row>
-    <row r="46" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -31097,7 +31097,7 @@
       <c r="FL46" s="11"/>
       <c r="FM46" s="11"/>
     </row>
-    <row r="47" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -31270,7 +31270,7 @@
       <c r="FL47" s="11"/>
       <c r="FM47" s="11"/>
     </row>
-    <row r="48" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -31443,7 +31443,7 @@
       <c r="FL48" s="11"/>
       <c r="FM48" s="11"/>
     </row>
-    <row r="49" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -31618,7 +31618,7 @@
       <c r="FL49" s="11"/>
       <c r="FM49" s="11"/>
     </row>
-    <row r="50" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="4"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -31799,7 +31799,7 @@
       <c r="FL50" s="11"/>
       <c r="FM50" s="11"/>
     </row>
-    <row r="51" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -31974,7 +31974,7 @@
       <c r="FL51" s="11"/>
       <c r="FM51" s="11"/>
     </row>
-    <row r="52" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -32147,7 +32147,7 @@
       <c r="FL52" s="11"/>
       <c r="FM52" s="11"/>
     </row>
-    <row r="53" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="4"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -32320,10 +32320,10 @@
       <c r="FL53" s="11"/>
       <c r="FM53" s="11"/>
     </row>
-    <row r="54" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" s="4"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="28" t="s">
         <v>658</v>
       </c>
       <c r="D54" s="13" t="s">
@@ -32497,7 +32497,7 @@
       <c r="FL54" s="11"/>
       <c r="FM54" s="11"/>
     </row>
-    <row r="55" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -32670,7 +32670,7 @@
       <c r="FL55" s="11"/>
       <c r="FM55" s="11"/>
     </row>
-    <row r="56" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -32843,7 +32843,7 @@
       <c r="FL56" s="11"/>
       <c r="FM56" s="11"/>
     </row>
-    <row r="57" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -33016,7 +33016,7 @@
       <c r="FL57" s="11"/>
       <c r="FM57" s="11"/>
     </row>
-    <row r="58" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -33189,7 +33189,7 @@
       <c r="FL58" s="11"/>
       <c r="FM58" s="11"/>
     </row>
-    <row r="59" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -33362,7 +33362,7 @@
       <c r="FL59" s="11"/>
       <c r="FM59" s="11"/>
     </row>
-    <row r="60" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -33537,7 +33537,7 @@
       <c r="FL60" s="11"/>
       <c r="FM60" s="11"/>
     </row>
-    <row r="61" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -33710,7 +33710,7 @@
       <c r="FL61" s="11"/>
       <c r="FM61" s="11"/>
     </row>
-    <row r="62" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A62" s="4"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -33893,7 +33893,7 @@
       <c r="FL62" s="11"/>
       <c r="FM62" s="11"/>
     </row>
-    <row r="63" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="4"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -34068,7 +34068,7 @@
       <c r="FL63" s="11"/>
       <c r="FM63" s="11"/>
     </row>
-    <row r="64" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -34247,7 +34247,7 @@
       <c r="FL64" s="11"/>
       <c r="FM64" s="11"/>
     </row>
-    <row r="65" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -34420,7 +34420,7 @@
       <c r="FL65" s="11"/>
       <c r="FM65" s="11"/>
     </row>
-    <row r="66" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="4"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -34595,7 +34595,7 @@
       <c r="FL66" s="11"/>
       <c r="FM66" s="11"/>
     </row>
-    <row r="67" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -34768,7 +34768,7 @@
       <c r="FL67" s="11"/>
       <c r="FM67" s="11"/>
     </row>
-    <row r="68" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -34941,10 +34941,10 @@
       <c r="FL68" s="11"/>
       <c r="FM68" s="11"/>
     </row>
-    <row r="69" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A69" s="4"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="31" t="s">
+      <c r="C69" s="28" t="s">
         <v>686</v>
       </c>
       <c r="D69" s="10" t="s">
@@ -35116,7 +35116,7 @@
       <c r="FL69" s="11"/>
       <c r="FM69" s="11"/>
     </row>
-    <row r="70" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A70" s="4"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -35295,7 +35295,7 @@
       <c r="FL70" s="11"/>
       <c r="FM70" s="11"/>
     </row>
-    <row r="71" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -35468,7 +35468,7 @@
       <c r="FL71" s="11"/>
       <c r="FM71" s="11"/>
     </row>
-    <row r="72" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A72" s="4"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -35641,7 +35641,7 @@
       <c r="FL72" s="11"/>
       <c r="FM72" s="11"/>
     </row>
-    <row r="73" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="4"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -35816,7 +35816,7 @@
       <c r="FL73" s="11"/>
       <c r="FM73" s="11"/>
     </row>
-    <row r="74" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -35995,7 +35995,7 @@
       <c r="FL74" s="11"/>
       <c r="FM74" s="11"/>
     </row>
-    <row r="75" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A75" s="4"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -36168,7 +36168,7 @@
       <c r="FL75" s="11"/>
       <c r="FM75" s="11"/>
     </row>
-    <row r="76" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="4"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -36341,7 +36341,7 @@
       <c r="FL76" s="11"/>
       <c r="FM76" s="11"/>
     </row>
-    <row r="77" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -36514,7 +36514,7 @@
       <c r="FL77" s="11"/>
       <c r="FM77" s="11"/>
     </row>
-    <row r="78" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -36687,7 +36687,7 @@
       <c r="FL78" s="11"/>
       <c r="FM78" s="11"/>
     </row>
-    <row r="79" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -36860,7 +36860,7 @@
       <c r="FL79" s="11"/>
       <c r="FM79" s="11"/>
     </row>
-    <row r="80" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -37033,7 +37033,7 @@
       <c r="FL80" s="11"/>
       <c r="FM80" s="11"/>
     </row>
-    <row r="81" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A81" s="4"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -37206,7 +37206,7 @@
       <c r="FL81" s="11"/>
       <c r="FM81" s="11"/>
     </row>
-    <row r="82" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -37381,7 +37381,7 @@
       <c r="FL82" s="11"/>
       <c r="FM82" s="11"/>
     </row>
-    <row r="83" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -37554,13 +37554,13 @@
       <c r="FL83" s="11"/>
       <c r="FM83" s="11"/>
     </row>
-    <row r="84" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
-      <c r="C84" s="32" t="s">
+      <c r="C84" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D84" s="33" t="s">
+      <c r="D84" s="30" t="s">
         <v>709</v>
       </c>
       <c r="E84" s="6"/>
@@ -37749,11 +37749,11 @@
       <c r="FL84" s="11"/>
       <c r="FM84" s="11"/>
     </row>
-    <row r="85" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A85" s="4"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="33" t="s">
+      <c r="D85" s="30" t="s">
         <v>716</v>
       </c>
       <c r="E85" s="6"/>
@@ -37934,11 +37934,11 @@
       <c r="FL85" s="11"/>
       <c r="FM85" s="11"/>
     </row>
-    <row r="86" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="33" t="s">
+      <c r="D86" s="30" t="s">
         <v>723</v>
       </c>
       <c r="E86" s="6"/>
@@ -38107,11 +38107,11 @@
       <c r="FL86" s="11"/>
       <c r="FM86" s="11"/>
     </row>
-    <row r="87" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="30" t="s">
         <v>724</v>
       </c>
       <c r="E87" s="6"/>
@@ -38286,11 +38286,11 @@
       <c r="FL87" s="11"/>
       <c r="FM87" s="11"/>
     </row>
-    <row r="88" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
-      <c r="D88" s="33" t="s">
+      <c r="D88" s="30" t="s">
         <v>728</v>
       </c>
       <c r="E88" s="6"/>
@@ -38459,10 +38459,10 @@
       <c r="FL88" s="11"/>
       <c r="FM88" s="11"/>
     </row>
-    <row r="89" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
-      <c r="C89" s="31" t="s">
+      <c r="C89" s="28" t="s">
         <v>729</v>
       </c>
       <c r="D89" s="13" t="s">
@@ -38634,7 +38634,7 @@
       <c r="FL89" s="11"/>
       <c r="FM89" s="11"/>
     </row>
-    <row r="90" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -38811,7 +38811,7 @@
       <c r="FL90" s="11"/>
       <c r="FM90" s="11"/>
     </row>
-    <row r="91" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -38984,7 +38984,7 @@
       <c r="FL91" s="11"/>
       <c r="FM91" s="11"/>
     </row>
-    <row r="92" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -39157,7 +39157,7 @@
       <c r="FL92" s="11"/>
       <c r="FM92" s="11"/>
     </row>
-    <row r="93" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -39330,7 +39330,7 @@
       <c r="FL93" s="11"/>
       <c r="FM93" s="11"/>
     </row>
-    <row r="94" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A94" s="4"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -39503,7 +39503,7 @@
       <c r="FL94" s="11"/>
       <c r="FM94" s="11"/>
     </row>
-    <row r="95" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -39676,7 +39676,7 @@
       <c r="FL95" s="11"/>
       <c r="FM95" s="11"/>
     </row>
-    <row r="96" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A96" s="4"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -39851,7 +39851,7 @@
       <c r="FL96" s="11"/>
       <c r="FM96" s="11"/>
     </row>
-    <row r="97" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="4"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -40026,7 +40026,7 @@
       <c r="FL97" s="11"/>
       <c r="FM97" s="11"/>
     </row>
-    <row r="98" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -40199,7 +40199,7 @@
       <c r="FL98" s="11"/>
       <c r="FM98" s="11"/>
     </row>
-    <row r="99" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A99" s="4"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -40372,7 +40372,7 @@
       <c r="FL99" s="11"/>
       <c r="FM99" s="11"/>
     </row>
-    <row r="100" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -40545,7 +40545,7 @@
       <c r="FL100" s="11"/>
       <c r="FM100" s="11"/>
     </row>
-    <row r="101" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -40718,7 +40718,7 @@
       <c r="FL101" s="11"/>
       <c r="FM101" s="11"/>
     </row>
-    <row r="102" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -40895,7 +40895,7 @@
       <c r="FL102" s="11"/>
       <c r="FM102" s="11"/>
     </row>
-    <row r="103" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -41068,13 +41068,13 @@
       <c r="FL103" s="11"/>
       <c r="FM103" s="11"/>
     </row>
-    <row r="104" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
-      <c r="C104" s="32" t="s">
+      <c r="C104" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D104" s="33" t="s">
+      <c r="D104" s="30" t="s">
         <v>750</v>
       </c>
       <c r="E104" s="6"/>
@@ -41259,11 +41259,11 @@
       <c r="FL104" s="11"/>
       <c r="FM104" s="11"/>
     </row>
-    <row r="105" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A105" s="4"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
-      <c r="D105" s="33" t="s">
+      <c r="D105" s="30" t="s">
         <v>757</v>
       </c>
       <c r="E105" s="6"/>
@@ -41448,11 +41448,11 @@
       <c r="FL105" s="11"/>
       <c r="FM105" s="11"/>
     </row>
-    <row r="106" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A106" s="4"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="33" t="s">
+      <c r="D106" s="30" t="s">
         <v>763</v>
       </c>
       <c r="E106" s="6"/>
@@ -41627,11 +41627,11 @@
       <c r="FL106" s="11"/>
       <c r="FM106" s="11"/>
     </row>
-    <row r="107" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A107" s="4"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
-      <c r="D107" s="33" t="s">
+      <c r="D107" s="30" t="s">
         <v>767</v>
       </c>
       <c r="E107" s="6"/>
@@ -41812,11 +41812,11 @@
       <c r="FL107" s="11"/>
       <c r="FM107" s="11"/>
     </row>
-    <row r="108" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="4"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
-      <c r="D108" s="33" t="s">
+      <c r="D108" s="30" t="s">
         <v>773</v>
       </c>
       <c r="E108" s="6"/>
@@ -42001,11 +42001,11 @@
       <c r="FL108" s="11"/>
       <c r="FM108" s="11"/>
     </row>
-    <row r="109" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A109" s="4"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
-      <c r="D109" s="33" t="s">
+      <c r="D109" s="30" t="s">
         <v>781</v>
       </c>
       <c r="E109" s="6"/>
@@ -42174,10 +42174,10 @@
       <c r="FL109" s="11"/>
       <c r="FM109" s="11"/>
     </row>
-    <row r="110" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="4"/>
       <c r="B110" s="5"/>
-      <c r="C110" s="31" t="s">
+      <c r="C110" s="28" t="s">
         <v>782</v>
       </c>
       <c r="D110" s="10" t="s">
@@ -42357,7 +42357,7 @@
       <c r="FL110" s="11"/>
       <c r="FM110" s="11"/>
     </row>
-    <row r="111" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A111" s="4"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
@@ -42530,7 +42530,7 @@
       <c r="FL111" s="11"/>
       <c r="FM111" s="11"/>
     </row>
-    <row r="112" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A112" s="4"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
@@ -42703,7 +42703,7 @@
       <c r="FL112" s="11"/>
       <c r="FM112" s="11"/>
     </row>
-    <row r="113" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A113" s="4"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -42878,7 +42878,7 @@
       <c r="FL113" s="11"/>
       <c r="FM113" s="11"/>
     </row>
-    <row r="114" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A114" s="4"/>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -43053,7 +43053,7 @@
       <c r="FL114" s="11"/>
       <c r="FM114" s="11"/>
     </row>
-    <row r="115" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="4"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
@@ -43226,7 +43226,7 @@
       <c r="FL115" s="11"/>
       <c r="FM115" s="11"/>
     </row>
-    <row r="116" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A116" s="4"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
@@ -43401,7 +43401,7 @@
       <c r="FL116" s="11"/>
       <c r="FM116" s="11"/>
     </row>
-    <row r="117" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A117" s="4"/>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
@@ -43574,7 +43574,7 @@
       <c r="FL117" s="11"/>
       <c r="FM117" s="11"/>
     </row>
-    <row r="118" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A118" s="4"/>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
@@ -43747,7 +43747,7 @@
       <c r="FL118" s="11"/>
       <c r="FM118" s="11"/>
     </row>
-    <row r="119" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A119" s="4"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
@@ -43920,7 +43920,7 @@
       <c r="FL119" s="11"/>
       <c r="FM119" s="11"/>
     </row>
-    <row r="120" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A120" s="4"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -44099,7 +44099,7 @@
       <c r="FL120" s="11"/>
       <c r="FM120" s="11"/>
     </row>
-    <row r="121" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A121" s="4"/>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
@@ -44290,7 +44290,7 @@
       <c r="FL121" s="11"/>
       <c r="FM121" s="11"/>
     </row>
-    <row r="122" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A122" s="4"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
@@ -44471,7 +44471,7 @@
       <c r="FL122" s="11"/>
       <c r="FM122" s="11"/>
     </row>
-    <row r="123" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A123" s="4"/>
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
@@ -44662,7 +44662,7 @@
       <c r="FL123" s="11"/>
       <c r="FM123" s="11"/>
     </row>
-    <row r="124" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A124" s="4"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
@@ -44835,10 +44835,10 @@
       <c r="FL124" s="11"/>
       <c r="FM124" s="11"/>
     </row>
-    <row r="125" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="4"/>
       <c r="B125" s="5"/>
-      <c r="C125" s="31" t="s">
+      <c r="C125" s="28" t="s">
         <v>826</v>
       </c>
       <c r="D125" s="13" t="s">
@@ -45010,7 +45010,7 @@
       <c r="FL125" s="11"/>
       <c r="FM125" s="11"/>
     </row>
-    <row r="126" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A126" s="4"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
@@ -45183,7 +45183,7 @@
       <c r="FL126" s="11"/>
       <c r="FM126" s="11"/>
     </row>
-    <row r="127" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A127" s="4"/>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
@@ -45356,7 +45356,7 @@
       <c r="FL127" s="11"/>
       <c r="FM127" s="11"/>
     </row>
-    <row r="128" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="4"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -45529,7 +45529,7 @@
       <c r="FL128" s="11"/>
       <c r="FM128" s="11"/>
     </row>
-    <row r="129" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A129" s="4"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -45702,7 +45702,7 @@
       <c r="FL129" s="11"/>
       <c r="FM129" s="11"/>
     </row>
-    <row r="130" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A130" s="4"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
@@ -45875,7 +45875,7 @@
       <c r="FL130" s="11"/>
       <c r="FM130" s="11"/>
     </row>
-    <row r="131" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A131" s="4"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
@@ -46054,7 +46054,7 @@
       <c r="FL131" s="11"/>
       <c r="FM131" s="11"/>
     </row>
-    <row r="132" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A132" s="4"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
@@ -46229,7 +46229,7 @@
       <c r="FL132" s="11"/>
       <c r="FM132" s="11"/>
     </row>
-    <row r="133" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A133" s="4"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
@@ -46402,7 +46402,7 @@
       <c r="FL133" s="11"/>
       <c r="FM133" s="11"/>
     </row>
-    <row r="134" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A134" s="4"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
@@ -46575,7 +46575,7 @@
       <c r="FL134" s="11"/>
       <c r="FM134" s="11"/>
     </row>
-    <row r="135" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A135" s="4"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
@@ -46752,7 +46752,7 @@
       <c r="FL135" s="11"/>
       <c r="FM135" s="11"/>
     </row>
-    <row r="136" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A136" s="4"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -46925,7 +46925,7 @@
       <c r="FL136" s="11"/>
       <c r="FM136" s="11"/>
     </row>
-    <row r="137" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A137" s="4"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
@@ -47104,7 +47104,7 @@
       <c r="FL137" s="11"/>
       <c r="FM137" s="11"/>
     </row>
-    <row r="138" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A138" s="4"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
@@ -47277,7 +47277,7 @@
       <c r="FL138" s="11"/>
       <c r="FM138" s="11"/>
     </row>
-    <row r="139" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="4"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -47450,10 +47450,10 @@
       <c r="FL139" s="11"/>
       <c r="FM139" s="11"/>
     </row>
-    <row r="140" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A140" s="4"/>
       <c r="B140" s="5"/>
-      <c r="C140" s="31" t="s">
+      <c r="C140" s="28" t="s">
         <v>849</v>
       </c>
       <c r="D140" s="10" t="s">
@@ -47633,7 +47633,7 @@
       <c r="FL140" s="11"/>
       <c r="FM140" s="11"/>
     </row>
-    <row r="141" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A141" s="4"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -47806,7 +47806,7 @@
       <c r="FL141" s="11"/>
       <c r="FM141" s="11"/>
     </row>
-    <row r="142" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A142" s="4"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -47981,7 +47981,7 @@
       <c r="FL142" s="11"/>
       <c r="FM142" s="11"/>
     </row>
-    <row r="143" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A143" s="4"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -48154,7 +48154,7 @@
       <c r="FL143" s="11"/>
       <c r="FM143" s="11"/>
     </row>
-    <row r="144" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A144" s="4"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
@@ -48331,7 +48331,7 @@
       <c r="FL144" s="11"/>
       <c r="FM144" s="11"/>
     </row>
-    <row r="145" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A145" s="4"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
@@ -48522,7 +48522,7 @@
       <c r="FL145" s="11"/>
       <c r="FM145" s="11"/>
     </row>
-    <row r="146" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A146" s="4"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
@@ -48695,7 +48695,7 @@
       <c r="FL146" s="11"/>
       <c r="FM146" s="11"/>
     </row>
-    <row r="147" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A147" s="4"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -48868,13 +48868,13 @@
       <c r="FL147" s="11"/>
       <c r="FM147" s="11"/>
     </row>
-    <row r="148" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A148" s="4"/>
       <c r="B148" s="5"/>
-      <c r="C148" s="32" t="s">
+      <c r="C148" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D148" s="33" t="s">
+      <c r="D148" s="30" t="s">
         <v>869</v>
       </c>
       <c r="E148" s="26"/>
@@ -49061,11 +49061,11 @@
       <c r="FL148" s="11"/>
       <c r="FM148" s="11"/>
     </row>
-    <row r="149" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="4"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
-      <c r="D149" s="33" t="s">
+      <c r="D149" s="30" t="s">
         <v>878</v>
       </c>
       <c r="E149" s="26"/>
@@ -49234,11 +49234,11 @@
       <c r="FL149" s="11"/>
       <c r="FM149" s="11"/>
     </row>
-    <row r="150" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A150" s="4"/>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
-      <c r="D150" s="33" t="s">
+      <c r="D150" s="30" t="s">
         <v>879</v>
       </c>
       <c r="E150" s="26"/>
@@ -49413,11 +49413,11 @@
       <c r="FL150" s="11"/>
       <c r="FM150" s="11"/>
     </row>
-    <row r="151" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A151" s="4"/>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
-      <c r="D151" s="33" t="s">
+      <c r="D151" s="30" t="s">
         <v>882</v>
       </c>
       <c r="E151" s="26"/>
@@ -49590,11 +49590,11 @@
       <c r="FL151" s="11"/>
       <c r="FM151" s="11"/>
     </row>
-    <row r="152" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A152" s="4"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
-      <c r="D152" s="33" t="s">
+      <c r="D152" s="30" t="s">
         <v>885</v>
       </c>
       <c r="E152" s="26"/>
@@ -49771,11 +49771,11 @@
       <c r="FL152" s="11"/>
       <c r="FM152" s="11"/>
     </row>
-    <row r="153" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A153" s="4"/>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
-      <c r="D153" s="33" t="s">
+      <c r="D153" s="30" t="s">
         <v>888</v>
       </c>
       <c r="E153" s="26"/>
@@ -49960,10 +49960,10 @@
       <c r="FL153" s="11"/>
       <c r="FM153" s="11"/>
     </row>
-    <row r="154" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
-      <c r="C154" s="31" t="s">
+      <c r="C154" s="28" t="s">
         <v>895</v>
       </c>
       <c r="D154" s="13" t="s">
@@ -50135,7 +50135,7 @@
       <c r="FL154" s="11"/>
       <c r="FM154" s="11"/>
     </row>
-    <row r="155" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
@@ -50314,7 +50314,7 @@
       <c r="FL155" s="11"/>
       <c r="FM155" s="11"/>
     </row>
-    <row r="156" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
@@ -50487,7 +50487,7 @@
       <c r="FL156" s="11"/>
       <c r="FM156" s="11"/>
     </row>
-    <row r="157" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
@@ -50662,7 +50662,7 @@
       <c r="FL157" s="11"/>
       <c r="FM157" s="11"/>
     </row>
-    <row r="158" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
@@ -50851,7 +50851,7 @@
       <c r="FL158" s="11"/>
       <c r="FM158" s="11"/>
     </row>
-    <row r="159" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
@@ -51028,7 +51028,7 @@
       <c r="FL159" s="11"/>
       <c r="FM159" s="11"/>
     </row>
-    <row r="160" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
@@ -51201,7 +51201,7 @@
       <c r="FL160" s="11"/>
       <c r="FM160" s="11"/>
     </row>
-    <row r="161" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
@@ -51374,13 +51374,13 @@
       <c r="FL161" s="11"/>
       <c r="FM161" s="11"/>
     </row>
-    <row r="162" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
-      <c r="C162" s="32" t="s">
+      <c r="C162" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D162" s="33" t="s">
+      <c r="D162" s="30" t="s">
         <v>916</v>
       </c>
       <c r="E162" s="26"/>
@@ -51573,11 +51573,11 @@
       <c r="FL162" s="11"/>
       <c r="FM162" s="11"/>
     </row>
-    <row r="163" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
-      <c r="D163" s="33" t="s">
+      <c r="D163" s="30" t="s">
         <v>927</v>
       </c>
       <c r="E163" s="26"/>
@@ -51746,11 +51746,11 @@
       <c r="FL163" s="11"/>
       <c r="FM163" s="11"/>
     </row>
-    <row r="164" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
-      <c r="D164" s="33" t="s">
+      <c r="D164" s="30" t="s">
         <v>928</v>
       </c>
       <c r="E164" s="26"/>
@@ -51931,11 +51931,11 @@
       <c r="FL164" s="11"/>
       <c r="FM164" s="11"/>
     </row>
-    <row r="165" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
-      <c r="D165" s="33" t="s">
+      <c r="D165" s="30" t="s">
         <v>933</v>
       </c>
       <c r="E165" s="26"/>
@@ -52112,11 +52112,11 @@
       <c r="FL165" s="11"/>
       <c r="FM165" s="11"/>
     </row>
-    <row r="166" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
-      <c r="D166" s="33" t="s">
+      <c r="D166" s="30" t="s">
         <v>937</v>
       </c>
       <c r="E166" s="26"/>
@@ -52287,11 +52287,11 @@
       <c r="FL166" s="11"/>
       <c r="FM166" s="11"/>
     </row>
-    <row r="167" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
-      <c r="D167" s="33" t="s">
+      <c r="D167" s="30" t="s">
         <v>939</v>
       </c>
       <c r="E167" s="26"/>
@@ -52462,10 +52462,10 @@
       <c r="FL167" s="11"/>
       <c r="FM167" s="11"/>
     </row>
-    <row r="168" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
-      <c r="C168" s="31" t="s">
+      <c r="C168" s="28" t="s">
         <v>940</v>
       </c>
       <c r="D168" s="10" t="s">
@@ -52637,7 +52637,7 @@
       <c r="FL168" s="11"/>
       <c r="FM168" s="11"/>
     </row>
-    <row r="169" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
@@ -52816,7 +52816,7 @@
       <c r="FL169" s="11"/>
       <c r="FM169" s="11"/>
     </row>
-    <row r="170" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
@@ -52989,7 +52989,7 @@
       <c r="FL170" s="11"/>
       <c r="FM170" s="11"/>
     </row>
-    <row r="171" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
@@ -53164,7 +53164,7 @@
       <c r="FL171" s="11"/>
       <c r="FM171" s="11"/>
     </row>
-    <row r="172" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -53337,7 +53337,7 @@
       <c r="FL172" s="11"/>
       <c r="FM172" s="11"/>
     </row>
-    <row r="173" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -53526,7 +53526,7 @@
       <c r="FL173" s="11"/>
       <c r="FM173" s="11"/>
     </row>
-    <row r="174" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -53703,7 +53703,7 @@
       <c r="FL174" s="11"/>
       <c r="FM174" s="11"/>
     </row>
-    <row r="175" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -53878,13 +53878,13 @@
       <c r="FL175" s="11"/>
       <c r="FM175" s="11"/>
     </row>
-    <row r="176" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
-      <c r="C176" s="32" t="s">
+      <c r="C176" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D176" s="33" t="s">
+      <c r="D176" s="30" t="s">
         <v>961</v>
       </c>
       <c r="E176" s="26"/>
@@ -54061,11 +54061,11 @@
       <c r="FL176" s="11"/>
       <c r="FM176" s="11"/>
     </row>
-    <row r="177" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
-      <c r="D177" s="33" t="s">
+      <c r="D177" s="30" t="s">
         <v>966</v>
       </c>
       <c r="E177" s="26"/>
@@ -54252,11 +54252,11 @@
       <c r="FL177" s="11"/>
       <c r="FM177" s="11"/>
     </row>
-    <row r="178" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
-      <c r="D178" s="33" t="s">
+      <c r="D178" s="30" t="s">
         <v>974</v>
       </c>
       <c r="E178" s="26"/>
@@ -54429,11 +54429,11 @@
       <c r="FL178" s="11"/>
       <c r="FM178" s="11"/>
     </row>
-    <row r="179" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
-      <c r="D179" s="33" t="s">
+      <c r="D179" s="30" t="s">
         <v>977</v>
       </c>
       <c r="E179" s="26"/>
@@ -54608,11 +54608,11 @@
       <c r="FL179" s="11"/>
       <c r="FM179" s="11"/>
     </row>
-    <row r="180" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
-      <c r="D180" s="33" t="s">
+      <c r="D180" s="30" t="s">
         <v>980</v>
       </c>
       <c r="E180" s="26"/>
@@ -54785,11 +54785,11 @@
       <c r="FL180" s="11"/>
       <c r="FM180" s="11"/>
     </row>
-    <row r="181" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
-      <c r="D181" s="33" t="s">
+      <c r="D181" s="30" t="s">
         <v>983</v>
       </c>
       <c r="E181" s="26"/>
@@ -54960,10 +54960,10 @@
       <c r="FL181" s="11"/>
       <c r="FM181" s="11"/>
     </row>
-    <row r="182" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="31" t="s">
+      <c r="C182" s="28" t="s">
         <v>985</v>
       </c>
       <c r="D182" s="13" t="s">
@@ -55135,7 +55135,7 @@
       <c r="FL182" s="11"/>
       <c r="FM182" s="11"/>
     </row>
-    <row r="183" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
@@ -55310,7 +55310,7 @@
       <c r="FL183" s="11"/>
       <c r="FM183" s="11"/>
     </row>
-    <row r="184" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
@@ -55483,7 +55483,7 @@
       <c r="FL184" s="11"/>
       <c r="FM184" s="11"/>
     </row>
-    <row r="185" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
@@ -55656,7 +55656,7 @@
       <c r="FL185" s="11"/>
       <c r="FM185" s="11"/>
     </row>
-    <row r="186" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
@@ -55829,7 +55829,7 @@
       <c r="FL186" s="11"/>
       <c r="FM186" s="11"/>
     </row>
-    <row r="187" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
@@ -56018,7 +56018,7 @@
       <c r="FL187" s="11"/>
       <c r="FM187" s="11"/>
     </row>
-    <row r="188" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
@@ -56191,7 +56191,7 @@
       <c r="FL188" s="11"/>
       <c r="FM188" s="11"/>
     </row>
-    <row r="189" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
@@ -56364,13 +56364,13 @@
       <c r="FL189" s="11"/>
       <c r="FM189" s="11"/>
     </row>
-    <row r="190" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
-      <c r="C190" s="32" t="s">
+      <c r="C190" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D190" s="33" t="s">
+      <c r="D190" s="30" t="s">
         <v>998</v>
       </c>
       <c r="E190" s="26"/>
@@ -56541,11 +56541,11 @@
       <c r="FL190" s="11"/>
       <c r="FM190" s="11"/>
     </row>
-    <row r="191" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
-      <c r="D191" s="33" t="s">
+      <c r="D191" s="30" t="s">
         <v>999</v>
       </c>
       <c r="E191" s="26"/>
@@ -56726,11 +56726,11 @@
       <c r="FL191" s="11"/>
       <c r="FM191" s="11"/>
     </row>
-    <row r="192" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
-      <c r="D192" s="33" t="s">
+      <c r="D192" s="30" t="s">
         <v>1004</v>
       </c>
       <c r="E192" s="26"/>
@@ -56909,11 +56909,11 @@
       <c r="FL192" s="11"/>
       <c r="FM192" s="11"/>
     </row>
-    <row r="193" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
-      <c r="D193" s="33" t="s">
+      <c r="D193" s="30" t="s">
         <v>1009</v>
       </c>
       <c r="E193" s="26"/>
@@ -57108,11 +57108,11 @@
       <c r="FL193" s="11"/>
       <c r="FM193" s="11"/>
     </row>
-    <row r="194" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
-      <c r="D194" s="33" t="s">
+      <c r="D194" s="30" t="s">
         <v>1023</v>
       </c>
       <c r="E194" s="26"/>
@@ -57281,11 +57281,11 @@
       <c r="FL194" s="11"/>
       <c r="FM194" s="11"/>
     </row>
-    <row r="195" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
-      <c r="D195" s="33" t="s">
+      <c r="D195" s="30" t="s">
         <v>1024</v>
       </c>
       <c r="E195" s="26"/>
@@ -57462,10 +57462,10 @@
       <c r="FL195" s="11"/>
       <c r="FM195" s="11"/>
     </row>
-    <row r="196" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
-      <c r="C196" s="31" t="s">
+      <c r="C196" s="28" t="s">
         <v>1029</v>
       </c>
       <c r="D196" s="10" t="s">
@@ -57637,7 +57637,7 @@
       <c r="FL196" s="11"/>
       <c r="FM196" s="11"/>
     </row>
-    <row r="197" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
@@ -57810,7 +57810,7 @@
       <c r="FL197" s="11"/>
       <c r="FM197" s="11"/>
     </row>
-    <row r="198" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
@@ -57983,7 +57983,7 @@
       <c r="FL198" s="11"/>
       <c r="FM198" s="11"/>
     </row>
-    <row r="199" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
@@ -58156,7 +58156,7 @@
       <c r="FL199" s="11"/>
       <c r="FM199" s="11"/>
     </row>
-    <row r="200" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
@@ -58331,7 +58331,7 @@
       <c r="FL200" s="11"/>
       <c r="FM200" s="11"/>
     </row>
-    <row r="201" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
@@ -58504,7 +58504,7 @@
       <c r="FL201" s="11"/>
       <c r="FM201" s="11"/>
     </row>
-    <row r="202" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
@@ -58679,7 +58679,7 @@
       <c r="FL202" s="11"/>
       <c r="FM202" s="11"/>
     </row>
-    <row r="203" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
@@ -58856,7 +58856,7 @@
       <c r="FL203" s="11"/>
       <c r="FM203" s="11"/>
     </row>
-    <row r="204" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
@@ -59029,7 +59029,7 @@
       <c r="FL204" s="11"/>
       <c r="FM204" s="11"/>
     </row>
-    <row r="205" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
@@ -59214,7 +59214,7 @@
       <c r="FL205" s="11"/>
       <c r="FM205" s="11"/>
     </row>
-    <row r="206" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
@@ -59387,7 +59387,7 @@
       <c r="FL206" s="11"/>
       <c r="FM206" s="11"/>
     </row>
-    <row r="207" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
@@ -59568,7 +59568,7 @@
       <c r="FL207" s="11"/>
       <c r="FM207" s="11"/>
     </row>
-    <row r="208" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
@@ -59743,7 +59743,7 @@
       <c r="FL208" s="11"/>
       <c r="FM208" s="11"/>
     </row>
-    <row r="209" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
@@ -59916,7 +59916,7 @@
       <c r="FL209" s="11"/>
       <c r="FM209" s="11"/>
     </row>
-    <row r="210" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
@@ -60089,13 +60089,13 @@
       <c r="FL210" s="11"/>
       <c r="FM210" s="11"/>
     </row>
-    <row r="211" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
-      <c r="C211" s="32" t="s">
+      <c r="C211" s="29" t="s">
         <v>600</v>
       </c>
-      <c r="D211" s="33" t="s">
+      <c r="D211" s="30" t="s">
         <v>1058</v>
       </c>
       <c r="E211" s="26"/>
@@ -60276,11 +60276,11 @@
       <c r="FL211" s="11"/>
       <c r="FM211" s="11"/>
     </row>
-    <row r="212" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
-      <c r="D212" s="33" t="s">
+      <c r="D212" s="30" t="s">
         <v>1063</v>
       </c>
       <c r="E212" s="26"/>
@@ -60453,11 +60453,11 @@
       <c r="FL212" s="11"/>
       <c r="FM212" s="11"/>
     </row>
-    <row r="213" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
-      <c r="D213" s="33" t="s">
+      <c r="D213" s="30" t="s">
         <v>1066</v>
       </c>
       <c r="E213" s="26"/>
@@ -60650,11 +60650,11 @@
       <c r="FL213" s="11"/>
       <c r="FM213" s="11"/>
     </row>
-    <row r="214" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
-      <c r="D214" s="33" t="s">
+      <c r="D214" s="30" t="s">
         <v>1077</v>
       </c>
       <c r="E214" s="26"/>
@@ -60843,11 +60843,11 @@
       <c r="FL214" s="11"/>
       <c r="FM214" s="11"/>
     </row>
-    <row r="215" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
-      <c r="D215" s="33" t="s">
+      <c r="D215" s="30" t="s">
         <v>1084</v>
       </c>
       <c r="E215" s="26"/>
@@ -61022,10 +61022,10 @@
       <c r="FL215" s="11"/>
       <c r="FM215" s="11"/>
     </row>
-    <row r="216" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
-      <c r="C216" s="31" t="s">
+      <c r="C216" s="28" t="s">
         <v>1088</v>
       </c>
       <c r="D216" s="13" t="s">
@@ -61211,7 +61211,7 @@
       <c r="FL216" s="11"/>
       <c r="FM216" s="11"/>
     </row>
-    <row r="217" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
@@ -61386,7 +61386,7 @@
       <c r="FL217" s="11"/>
       <c r="FM217" s="11"/>
     </row>
-    <row r="218" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
@@ -61559,7 +61559,7 @@
       <c r="FL218" s="11"/>
       <c r="FM218" s="11"/>
     </row>
-    <row r="219" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
@@ -61732,7 +61732,7 @@
       <c r="FL219" s="11"/>
       <c r="FM219" s="11"/>
     </row>
-    <row r="220" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
@@ -61909,7 +61909,7 @@
       <c r="FL220" s="11"/>
       <c r="FM220" s="11"/>
     </row>
-    <row r="221" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
@@ -62082,7 +62082,7 @@
       <c r="FL221" s="11"/>
       <c r="FM221" s="11"/>
     </row>
-    <row r="222" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
@@ -62257,7 +62257,7 @@
       <c r="FL222" s="11"/>
       <c r="FM222" s="11"/>
     </row>
-    <row r="223" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
@@ -62430,7 +62430,7 @@
       <c r="FL223" s="11"/>
       <c r="FM223" s="11"/>
     </row>
-    <row r="224" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
@@ -62603,7 +62603,7 @@
       <c r="FL224" s="11"/>
       <c r="FM224" s="11"/>
     </row>
-    <row r="225" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
@@ -62786,7 +62786,7 @@
       <c r="FL225" s="11"/>
       <c r="FM225" s="11"/>
     </row>
-    <row r="226" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
@@ -62961,7 +62961,7 @@
       <c r="FL226" s="11"/>
       <c r="FM226" s="11"/>
     </row>
-    <row r="227" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
@@ -63136,7 +63136,7 @@
       <c r="FL227" s="11"/>
       <c r="FM227" s="11"/>
     </row>
-    <row r="228" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
@@ -63309,13 +63309,13 @@
       <c r="FL228" s="11"/>
       <c r="FM228" s="11"/>
     </row>
-    <row r="229" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
-      <c r="C229" s="32" t="s">
+      <c r="C229" s="29" t="s">
         <v>1116</v>
       </c>
-      <c r="D229" s="33" t="s">
+      <c r="D229" s="30" t="s">
         <v>1117</v>
       </c>
       <c r="E229" s="26"/>
@@ -63508,11 +63508,11 @@
       <c r="FL229" s="11"/>
       <c r="FM229" s="11"/>
     </row>
-    <row r="230" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
-      <c r="D230" s="33" t="s">
+      <c r="D230" s="30" t="s">
         <v>1125</v>
       </c>
       <c r="E230" s="26"/>
@@ -63697,11 +63697,11 @@
       <c r="FL230" s="11"/>
       <c r="FM230" s="11"/>
     </row>
-    <row r="231" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
       <c r="C231" s="5"/>
-      <c r="D231" s="33" t="s">
+      <c r="D231" s="30" t="s">
         <v>1132</v>
       </c>
       <c r="E231" s="26"/>
@@ -63884,11 +63884,11 @@
       <c r="FL231" s="11"/>
       <c r="FM231" s="11"/>
     </row>
-    <row r="232" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
       <c r="C232" s="5"/>
-      <c r="D232" s="33" t="s">
+      <c r="D232" s="30" t="s">
         <v>1140</v>
       </c>
       <c r="E232" s="26"/>
@@ -64057,11 +64057,11 @@
       <c r="FL232" s="11"/>
       <c r="FM232" s="11"/>
     </row>
-    <row r="233" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
       <c r="C233" s="5"/>
-      <c r="D233" s="33" t="s">
+      <c r="D233" s="30" t="s">
         <v>1141</v>
       </c>
       <c r="E233" s="26"/>
@@ -64236,13 +64236,13 @@
       <c r="FL233" s="11"/>
       <c r="FM233" s="11"/>
     </row>
-    <row r="234" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
-      <c r="C234" s="32" t="s">
+      <c r="C234" s="29" t="s">
         <v>1144</v>
       </c>
-      <c r="D234" s="33" t="s">
+      <c r="D234" s="30" t="s">
         <v>1145</v>
       </c>
       <c r="E234" s="26"/>
@@ -64413,10 +64413,10 @@
       <c r="FL234" s="11"/>
       <c r="FM234" s="11"/>
     </row>
-    <row r="235" spans="1:169" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:169" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
-      <c r="C235" s="34" t="s">
+      <c r="C235" s="31" t="s">
         <v>1147</v>
       </c>
       <c r="D235" s="10" t="s">
@@ -64590,7 +64590,7 @@
       <c r="FL235" s="11"/>
       <c r="FM235" s="11"/>
     </row>
-    <row r="236" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
@@ -64769,7 +64769,7 @@
       <c r="FL236" s="11"/>
       <c r="FM236" s="11"/>
     </row>
-    <row r="237" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
       <c r="C237" s="5"/>
@@ -64970,7 +64970,7 @@
       <c r="FL237" s="11"/>
       <c r="FM237" s="11"/>
     </row>
-    <row r="238" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
@@ -65169,7 +65169,7 @@
       <c r="FL238" s="11"/>
       <c r="FM238" s="11"/>
     </row>
-    <row r="239" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
@@ -65346,7 +65346,7 @@
       <c r="FL239" s="11"/>
       <c r="FM239" s="11"/>
     </row>
-    <row r="240" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A240" s="4"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
@@ -65545,7 +65545,7 @@
       <c r="FL240" s="11"/>
       <c r="FM240" s="11"/>
     </row>
-    <row r="241" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A241" s="4"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
@@ -65718,7 +65718,7 @@
       <c r="FL241" s="11"/>
       <c r="FM241" s="11"/>
     </row>
-    <row r="242" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A242" s="4"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
@@ -65901,7 +65901,7 @@
       <c r="FL242" s="11"/>
       <c r="FM242" s="11"/>
     </row>
-    <row r="243" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A243" s="4"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
@@ -66088,7 +66088,7 @@
       <c r="FL243" s="11"/>
       <c r="FM243" s="11"/>
     </row>
-    <row r="244" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A244" s="4"/>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -66263,7 +66263,7 @@
       <c r="FL244" s="11"/>
       <c r="FM244" s="11"/>
     </row>
-    <row r="245" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A245" s="4"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
@@ -66456,7 +66456,7 @@
       <c r="FL245" s="11"/>
       <c r="FM245" s="11"/>
     </row>
-    <row r="246" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A246" s="4"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
@@ -66657,7 +66657,7 @@
       <c r="FL246" s="11"/>
       <c r="FM246" s="11"/>
     </row>
-    <row r="247" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A247" s="4"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
@@ -66828,7 +66828,7 @@
       <c r="FL247" s="11"/>
       <c r="FM247" s="11"/>
     </row>
-    <row r="248" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A248" s="4"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
@@ -66999,7 +66999,7 @@
       <c r="FL248" s="11"/>
       <c r="FM248" s="11"/>
     </row>
-    <row r="249" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A249" s="4"/>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -67170,7 +67170,7 @@
       <c r="FL249" s="11"/>
       <c r="FM249" s="11"/>
     </row>
-    <row r="250" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A250" s="4"/>
       <c r="B250" s="5"/>
       <c r="C250" s="5"/>
@@ -67341,7 +67341,7 @@
       <c r="FL250" s="11"/>
       <c r="FM250" s="11"/>
     </row>
-    <row r="251" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A251" s="4"/>
       <c r="B251" s="5"/>
       <c r="C251" s="5"/>
@@ -67512,7 +67512,7 @@
       <c r="FL251" s="11"/>
       <c r="FM251" s="11"/>
     </row>
-    <row r="252" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:169" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A252" s="4"/>
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
@@ -67683,7 +67683,7 @@
       <c r="FL252" s="26"/>
       <c r="FM252" s="26"/>
     </row>
-    <row r="253" spans="1:169" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:169" ht="154.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A253" s="27" t="s">
         <v>551</v>
       </c>

</xml_diff>